<commit_message>
Final attendance sheet changes
</commit_message>
<xml_diff>
--- a/backend/facerecog/Attendance.xlsx
+++ b/backend/facerecog/Attendance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>2023-03-28</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Attendance percentage</t>
   </si>
   <si>
     <t>cr07</t>
@@ -410,13 +416,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,105 +441,141 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>9</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>